<commit_message>
FINALLY finshed lab 6
</commit_message>
<xml_diff>
--- a/Mitchell_Lab6/TimingCSV.xlsx
+++ b/Mitchell_Lab6/TimingCSV.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="TimingCSV" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="170">
   <si>
     <t xml:space="preserve">BST Insert for n = 50000 and Seed = 1 Time = </t>
   </si>
@@ -513,31 +513,22 @@
     <t>n</t>
   </si>
   <si>
-    <t>BST Insert and Delete</t>
-  </si>
-  <si>
-    <t>2-3 Tree Insert</t>
-  </si>
-  <si>
-    <t>2-3 Tree Insert and Delete</t>
-  </si>
-  <si>
     <t>BST</t>
   </si>
   <si>
     <t>2-3 Tree</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>BST Insert (s)</t>
+  </si>
+  <si>
+    <t>BST Insert and Delete (s)</t>
+  </si>
+  <si>
+    <t>2-3 Tree Insert (s)</t>
+  </si>
+  <si>
+    <t>2-3 Tree Insert and Delete (s)</t>
   </si>
 </sst>
 </file>
@@ -1021,9 +1012,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1236,33 +1230,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$2:$D$9</c:f>
+              <c:f>TimingCSV!$D$14:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150000</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200000</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250000</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300000</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>350000</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>400000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,33 +1336,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>TimingCSV!$D$2:$D$9</c:f>
+              <c:f>TimingCSV!$D$14:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150000</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200000</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250000</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300000</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>350000</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>400000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,11 +1377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1818140560"/>
-        <c:axId val="1818147632"/>
+        <c:axId val="-1389653344"/>
+        <c:axId val="-1389641920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1818140560"/>
+        <c:axId val="-1389653344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,12 +1499,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1818147632"/>
+        <c:crossAx val="-1389641920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1818147632"/>
+        <c:axId val="-1389641920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1818140560"/>
+        <c:crossAx val="-1389653344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2005,11 +1999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2089820192"/>
-        <c:axId val="2082182208"/>
+        <c:axId val="-1389644640"/>
+        <c:axId val="-1389644096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2089820192"/>
+        <c:axId val="-1389644640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2122,12 +2116,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082182208"/>
+        <c:crossAx val="-1389644096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2082182208"/>
+        <c:axId val="-1389644096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,7 +2239,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2089820192"/>
+        <c:crossAx val="-1389644640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3442,16 +3436,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733426</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3472,16 +3466,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>414337</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3769,18 +3763,18 @@
   <dimension ref="A1:L160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D1" sqref="D1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3790,20 +3784,20 @@
       <c r="B1">
         <v>2.0739E-2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>163</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
         <v>162</v>
@@ -4057,16 +4051,16 @@
         <v>6.2933000000000003E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4092,6 +4086,10 @@
       <c r="B14">
         <v>3.7599999999999998E-4</v>
       </c>
+      <c r="D14">
+        <f>0.1*D2</f>
+        <v>5000</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -4100,6 +4098,10 @@
       <c r="B15">
         <v>6.2545000000000003E-2</v>
       </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D21" si="1">0.1*D3</f>
+        <v>10000</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4108,48 +4110,72 @@
       <c r="B16">
         <v>4.9600000000000002E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>2.9947999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>3.8000000000000002E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>6.3602000000000006E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>4.8899999999999996E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>0.1*D8</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>6.3238000000000003E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -4157,7 +4183,7 @@
         <v>7.6900000000000004E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -4165,7 +4191,7 @@
         <v>0.13969200000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -4173,7 +4199,7 @@
         <v>1.0280000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -4181,7 +4207,7 @@
         <v>7.3855000000000004E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4189,7 +4215,7 @@
         <v>7.45E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -4197,7 +4223,7 @@
         <v>0.152285</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4205,7 +4231,7 @@
         <v>1.021E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -4213,7 +4239,7 @@
         <v>7.4822E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4221,7 +4247,7 @@
         <v>7.5299999999999998E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4229,7 +4255,7 @@
         <v>0.15412899999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>

</xml_diff>